<commit_message>
31-07-2018 : Bugfixed ->frmMastEmpBasicData->Add Employee
</commit_message>
<xml_diff>
--- a/upload_template/EmpMaster_Upload.xlsx
+++ b/upload_template/EmpMaster_Upload.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SourceCode\Visual Studio 2013\Attendance-Kosi\Attendance - Kosi - JSAW\upload_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SourceCode\Visual Studio 2013\Attendance-NKP\upload_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="67">
   <si>
     <t>EmpUnqID</t>
   </si>
@@ -215,12 +215,18 @@
   </si>
   <si>
     <t>NRG</t>
+  </si>
+  <si>
+    <t>SPLALL</t>
+  </si>
+  <si>
+    <t>BAALL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -309,8 +315,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -609,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +676,7 @@
     <col min="31" max="31" width="28.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -739,8 +773,14 @@
       <c r="AF1" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9999999</v>
       </c>
@@ -825,8 +865,14 @@
       <c r="AF2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9999999</v>
       </c>
@@ -913,6 +959,12 @@
       </c>
       <c r="AF3">
         <v>320</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>